<commit_message>
codes for extent report is added
</commit_message>
<xml_diff>
--- a/target/test-classes/ownAssignments/WebTable.xlsx
+++ b/target/test-classes/ownAssignments/WebTable.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Company</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Italy</t>
+  </si>
+  <si>
+    <t>sasdsfads</t>
   </si>
 </sst>
 </file>
@@ -497,8 +500,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>5666.99</v>
+      <c r="A1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made corrections in ExtendReportPractice class
</commit_message>
<xml_diff>
--- a/target/test-classes/ownAssignments/WebTable.xlsx
+++ b/target/test-classes/ownAssignments/WebTable.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Company</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>Italy</t>
+  </si>
+  <si>
+    <t>sasdsfads</t>
   </si>
 </sst>
 </file>
@@ -497,8 +500,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>5666.99</v>
+      <c r="A1" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>